<commit_message>
Filter has been added!
</commit_message>
<xml_diff>
--- a/enteries.xlsx
+++ b/enteries.xlsx
@@ -14,27 +14,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Maxsulot nomi</t>
-  </si>
-  <si>
-    <t>Maxsulot soni</t>
-  </si>
-  <si>
-    <t>Maxsulot qo'shilgan sana</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>product_name</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>added_quantity</t>
+  </si>
+  <si>
+    <t>added_time</t>
   </si>
   <si>
     <t>Futbolka</t>
   </si>
   <si>
-    <t>BYD Atto 3</t>
+    <t>Redmi</t>
   </si>
   <si>
     <t>2024-02-09 00:55:55</t>
   </si>
   <si>
-    <t>2024-02-09 12:28:58</t>
+    <t>2024-02-13 10:13:06</t>
   </si>
 </sst>
 </file>
@@ -392,13 +395,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -408,27 +411,36 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
       <c r="B3">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>